<commit_message>
Modificacion en las fechas establecidas
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B142FA07-8BCD-4A11-9A32-7056E9C8C3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EE6070-D617-48E5-B7FF-FDE278AC0077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="591" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>INICIO</t>
-  </si>
-  <si>
-    <t>fecha</t>
   </si>
   <si>
     <t>FIN</t>
@@ -1382,9 +1379,6 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1393,6 +1387,12 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1417,9 +1417,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2302,11 +2299,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DB53"/>
+  <dimension ref="A1:DB52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2327,11 +2324,11 @@
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="B1" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="H1" s="1"/>
@@ -2341,10 +2338,10 @@
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="103"/>
+      <c r="B2" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="94"/>
       <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2352,164 +2349,164 @@
         <v>2</v>
       </c>
       <c r="B3" s="71"/>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="95">
+      <c r="D3" s="101"/>
+      <c r="E3" s="96">
         <f>DATE(2022,9,15)</f>
         <v>44819</v>
       </c>
-      <c r="F3" s="95"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="102"/>
+      <c r="D4" s="103"/>
       <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="96" t="s">
+      <c r="I4" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="96" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="98"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="98"/>
-      <c r="W4" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="92">
+      <c r="X4" s="98"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
         <v>44837</v>
       </c>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="93"/>
-      <c r="AJ4" s="94"/>
-      <c r="AK4" s="92">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
         <v>44844</v>
       </c>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="93"/>
-      <c r="AN4" s="93"/>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="94"/>
-      <c r="AR4" s="92">
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
         <v>44851</v>
       </c>
-      <c r="AS4" s="93"/>
-      <c r="AT4" s="93"/>
-      <c r="AU4" s="93"/>
-      <c r="AV4" s="93"/>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="94"/>
-      <c r="AY4" s="92">
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
         <v>44858</v>
       </c>
-      <c r="AZ4" s="93"/>
-      <c r="BA4" s="93"/>
-      <c r="BB4" s="93"/>
-      <c r="BC4" s="93"/>
-      <c r="BD4" s="93"/>
-      <c r="BE4" s="94"/>
-      <c r="BF4" s="92">
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
         <v>44865</v>
       </c>
-      <c r="BG4" s="93"/>
-      <c r="BH4" s="93"/>
-      <c r="BI4" s="93"/>
-      <c r="BJ4" s="93"/>
-      <c r="BK4" s="93"/>
-      <c r="BL4" s="94"/>
-      <c r="BM4" s="92">
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="91">
         <f>BM5</f>
         <v>44872</v>
       </c>
-      <c r="BN4" s="93"/>
-      <c r="BO4" s="93"/>
-      <c r="BP4" s="93"/>
-      <c r="BQ4" s="93"/>
-      <c r="BR4" s="93"/>
-      <c r="BS4" s="94"/>
-      <c r="BT4" s="92">
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="92"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="91">
         <f>BT5</f>
         <v>44879</v>
       </c>
-      <c r="BU4" s="93"/>
-      <c r="BV4" s="93"/>
-      <c r="BW4" s="93"/>
-      <c r="BX4" s="93"/>
-      <c r="BY4" s="93"/>
-      <c r="BZ4" s="94"/>
-      <c r="CA4" s="92">
+      <c r="BU4" s="92"/>
+      <c r="BV4" s="92"/>
+      <c r="BW4" s="92"/>
+      <c r="BX4" s="92"/>
+      <c r="BY4" s="92"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="91">
         <f>CA5</f>
         <v>44886</v>
       </c>
-      <c r="CB4" s="93"/>
-      <c r="CC4" s="93"/>
-      <c r="CD4" s="93"/>
-      <c r="CE4" s="93"/>
-      <c r="CF4" s="93"/>
-      <c r="CG4" s="94"/>
-      <c r="CH4" s="92">
+      <c r="CB4" s="92"/>
+      <c r="CC4" s="92"/>
+      <c r="CD4" s="92"/>
+      <c r="CE4" s="92"/>
+      <c r="CF4" s="92"/>
+      <c r="CG4" s="93"/>
+      <c r="CH4" s="91">
         <f>CH5</f>
         <v>44893</v>
       </c>
-      <c r="CI4" s="93"/>
-      <c r="CJ4" s="93"/>
-      <c r="CK4" s="93"/>
-      <c r="CL4" s="93"/>
-      <c r="CM4" s="93"/>
-      <c r="CN4" s="94"/>
-      <c r="CO4" s="92">
+      <c r="CI4" s="92"/>
+      <c r="CJ4" s="92"/>
+      <c r="CK4" s="92"/>
+      <c r="CL4" s="92"/>
+      <c r="CM4" s="92"/>
+      <c r="CN4" s="93"/>
+      <c r="CO4" s="91">
         <f>CO5</f>
         <v>44900</v>
       </c>
-      <c r="CP4" s="93"/>
-      <c r="CQ4" s="93"/>
-      <c r="CR4" s="93"/>
-      <c r="CS4" s="93"/>
-      <c r="CT4" s="93"/>
-      <c r="CU4" s="94"/>
-      <c r="CV4" s="92">
+      <c r="CP4" s="92"/>
+      <c r="CQ4" s="92"/>
+      <c r="CR4" s="92"/>
+      <c r="CS4" s="92"/>
+      <c r="CT4" s="92"/>
+      <c r="CU4" s="93"/>
+      <c r="CV4" s="91">
         <f>CV5</f>
         <v>44907</v>
       </c>
-      <c r="CW4" s="93"/>
-      <c r="CX4" s="93"/>
-      <c r="CY4" s="93"/>
-      <c r="CZ4" s="93"/>
-      <c r="DA4" s="93"/>
-      <c r="DB4" s="94"/>
+      <c r="CW4" s="92"/>
+      <c r="CX4" s="92"/>
+      <c r="CY4" s="92"/>
+      <c r="CZ4" s="92"/>
+      <c r="DA4" s="92"/>
+      <c r="DB4" s="93"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
@@ -2931,11 +2928,11 @@
         <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" ref="I6" si="33">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -3402,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="8"/>
@@ -3410,7 +3407,7 @@
       <c r="F8" s="46"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="str">
-        <f t="shared" ref="H8:H53" si="42">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H52" si="42">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="17"/>
@@ -3517,10 +3514,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="35" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>41</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -3642,10 +3639,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
@@ -3765,13 +3762,13 @@
     <row r="11" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="9">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E11" s="57">
         <f>F10</f>
@@ -3888,10 +3885,10 @@
     <row r="12" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
@@ -4011,13 +4008,13 @@
     <row r="13" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E13" s="57">
         <f>E10+32</f>
@@ -4136,7 +4133,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="10"/>
@@ -4249,10 +4246,10 @@
     <row r="15" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="70" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>51</v>
       </c>
       <c r="D15" s="11">
         <v>1</v>
@@ -4372,10 +4369,10 @@
     <row r="16" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16" s="63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="11">
         <v>1</v>
@@ -4495,10 +4492,10 @@
     <row r="17" spans="1:106" s="2" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="11">
         <v>0.7</v>
@@ -4618,10 +4615,10 @@
     <row r="18" spans="1:106" s="2" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="11">
         <v>1</v>
@@ -4741,10 +4738,10 @@
     <row r="19" spans="1:106" s="2" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
@@ -4866,7 +4863,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="39"/>
       <c r="D20" s="14"/>
@@ -4979,26 +4976,26 @@
     <row r="21" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
       <c r="B21" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="90" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="15">
         <v>0.5</v>
       </c>
       <c r="E21" s="59">
-        <f>BI5</f>
-        <v>44868</v>
+        <f>BM5</f>
+        <v>44872</v>
       </c>
       <c r="F21" s="59">
-        <f>BS5+1</f>
-        <v>44879</v>
+        <f>BZ5</f>
+        <v>44885</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
         <f t="shared" si="42"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -5102,10 +5099,10 @@
     <row r="22" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="15">
         <v>0</v>
@@ -5115,13 +5112,13 @@
         <v>44872</v>
       </c>
       <c r="F22" s="59">
-        <f>BS5+2</f>
-        <v>44880</v>
+        <f>BZ5</f>
+        <v>44885</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
         <f t="shared" si="42"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -5225,26 +5222,26 @@
     <row r="23" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="15">
         <v>0</v>
       </c>
       <c r="E23" s="59">
-        <f>AV5</f>
-        <v>44855</v>
+        <f>BZ5</f>
+        <v>44885</v>
       </c>
       <c r="F23" s="59">
-        <f>AW5</f>
-        <v>44856</v>
+        <f>CG5</f>
+        <v>44892</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
         <f t="shared" si="42"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -5350,7 +5347,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="12"/>
@@ -5463,10 +5460,10 @@
     <row r="25" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="13">
         <v>0</v>
@@ -5586,10 +5583,10 @@
     <row r="26" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="13">
         <v>0</v>
@@ -5709,10 +5706,10 @@
     <row r="27" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="13">
         <v>0</v>
@@ -5832,7 +5829,7 @@
     <row r="28" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
       <c r="B28" s="65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="13">
@@ -5953,7 +5950,7 @@
     <row r="29" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29" s="65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="38"/>
       <c r="D29" s="13">
@@ -6076,7 +6073,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="73"/>
       <c r="D30" s="74"/>
@@ -6191,24 +6188,24 @@
         <v>13</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="78"/>
       <c r="D31" s="79">
         <v>0</v>
       </c>
       <c r="E31" s="80">
-        <f>BT7</f>
-        <v>0</v>
+        <f>CO5</f>
+        <v>44900</v>
       </c>
       <c r="F31" s="80">
-        <f>BT7</f>
-        <v>0</v>
+        <f>CV5</f>
+        <v>44907</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="16">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -6311,24 +6308,24 @@
     </row>
     <row r="32" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="77" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="79">
         <v>0</v>
       </c>
       <c r="E32" s="80">
-        <f>BU7</f>
-        <v>0</v>
+        <f>CO5</f>
+        <v>44900</v>
       </c>
       <c r="F32" s="80">
-        <f>BV7</f>
-        <v>0</v>
+        <f>CV5</f>
+        <v>44907</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -6431,24 +6428,24 @@
     </row>
     <row r="33" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="78"/>
       <c r="D33" s="79">
         <v>0</v>
       </c>
       <c r="E33" s="80">
-        <f>BV7</f>
-        <v>0</v>
+        <f>CO5</f>
+        <v>44900</v>
       </c>
       <c r="F33" s="80">
-        <f>BW7</f>
-        <v>0</v>
+        <f>CV5</f>
+        <v>44907</v>
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="16">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -6551,24 +6548,24 @@
     </row>
     <row r="34" spans="2:106" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="78"/>
       <c r="D34" s="79">
         <v>0</v>
       </c>
       <c r="E34" s="80">
-        <f>BW7+1</f>
-        <v>1</v>
+        <f>CO5</f>
+        <v>44900</v>
       </c>
       <c r="F34" s="80">
-        <f>BX7+2</f>
-        <v>2</v>
+        <f>CV5</f>
+        <v>44907</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="16">
         <f t="shared" si="42"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -6670,21 +6667,17 @@
       <c r="DB34" s="17"/>
     </row>
     <row r="35" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="77"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="79">
-        <v>0</v>
-      </c>
-      <c r="E35" s="80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="80" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="16" t="e">
+      <c r="H35" s="16" t="str">
         <f t="shared" si="42"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -6786,17 +6779,25 @@
       <c r="DB35" s="17"/>
     </row>
     <row r="36" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="81" t="s">
+      <c r="B36" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="85"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="88">
+        <v>0</v>
+      </c>
+      <c r="E36" s="89">
+        <f>CW5</f>
+        <v>44908</v>
+      </c>
+      <c r="F36" s="89">
+        <f>CX5</f>
+        <v>44909</v>
+      </c>
       <c r="G36" s="16"/>
-      <c r="H36" s="16" t="str">
+      <c r="H36" s="16">
         <f t="shared" si="42"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -6898,25 +6899,17 @@
       <c r="DB36" s="17"/>
     </row>
     <row r="37" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="88">
-        <v>0</v>
-      </c>
-      <c r="E37" s="89">
-        <f>CA7</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="89">
-        <f>CG7</f>
-        <v>0</v>
-      </c>
+      <c r="B37" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="16">
+      <c r="H37" s="16" t="str">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
@@ -7018,17 +7011,25 @@
       <c r="DB37" s="17"/>
     </row>
     <row r="38" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="66" t="s">
+      <c r="B38" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="53"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="15">
+        <v>0</v>
+      </c>
+      <c r="E38" s="59">
+        <f>CW5</f>
+        <v>44908</v>
+      </c>
+      <c r="F38" s="59">
+        <f>CX5</f>
+        <v>44909</v>
+      </c>
       <c r="G38" s="16"/>
-      <c r="H38" s="16" t="str">
+      <c r="H38" s="16">
         <f t="shared" si="42"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
@@ -7130,25 +7131,10 @@
       <c r="DB38" s="17"/>
     </row>
     <row r="39" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="15">
-        <v>0</v>
-      </c>
-      <c r="E39" s="59">
-        <f>CX5</f>
-        <v>44909</v>
-      </c>
-      <c r="F39" s="59">
-        <f>CX5</f>
-        <v>44909</v>
-      </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="16">
+      <c r="H39" s="16" t="str">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
@@ -8614,113 +8600,11 @@
       <c r="DA52" s="17"/>
       <c r="DB52" s="17"/>
     </row>
-    <row r="53" spans="7:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="16"/>
-      <c r="H53" s="16" t="str">
-        <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="19"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="19"/>
-      <c r="W53" s="19"/>
-      <c r="X53" s="19"/>
-      <c r="Y53" s="19"/>
-      <c r="Z53" s="19"/>
-      <c r="AA53" s="19"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="19"/>
-      <c r="AD53" s="19"/>
-      <c r="AE53" s="19"/>
-      <c r="AF53" s="19"/>
-      <c r="AG53" s="19"/>
-      <c r="AH53" s="19"/>
-      <c r="AI53" s="19"/>
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-      <c r="AL53" s="19"/>
-      <c r="AM53" s="19"/>
-      <c r="AN53" s="19"/>
-      <c r="AO53" s="19"/>
-      <c r="AP53" s="19"/>
-      <c r="AQ53" s="19"/>
-      <c r="AR53" s="19"/>
-      <c r="AS53" s="19"/>
-      <c r="AT53" s="19"/>
-      <c r="AU53" s="19"/>
-      <c r="AV53" s="19"/>
-      <c r="AW53" s="19"/>
-      <c r="AX53" s="19"/>
-      <c r="AY53" s="19"/>
-      <c r="AZ53" s="19"/>
-      <c r="BA53" s="19"/>
-      <c r="BB53" s="19"/>
-      <c r="BC53" s="19"/>
-      <c r="BD53" s="19"/>
-      <c r="BE53" s="19"/>
-      <c r="BF53" s="19"/>
-      <c r="BG53" s="19"/>
-      <c r="BH53" s="19"/>
-      <c r="BI53" s="19"/>
-      <c r="BJ53" s="19"/>
-      <c r="BK53" s="19"/>
-      <c r="BL53" s="19"/>
-      <c r="BM53" s="17"/>
-      <c r="BN53" s="17"/>
-      <c r="BO53" s="17"/>
-      <c r="BP53" s="17"/>
-      <c r="BQ53" s="17"/>
-      <c r="BR53" s="17"/>
-      <c r="BS53" s="17"/>
-      <c r="BT53" s="17"/>
-      <c r="BU53" s="17"/>
-      <c r="BV53" s="17"/>
-      <c r="BW53" s="17"/>
-      <c r="BX53" s="17"/>
-      <c r="BY53" s="17"/>
-      <c r="BZ53" s="17"/>
-      <c r="CA53" s="17"/>
-      <c r="CB53" s="17"/>
-      <c r="CC53" s="17"/>
-      <c r="CD53" s="17"/>
-      <c r="CE53" s="17"/>
-      <c r="CF53" s="17"/>
-      <c r="CG53" s="17"/>
-      <c r="CH53" s="17"/>
-      <c r="CI53" s="17"/>
-      <c r="CJ53" s="17"/>
-      <c r="CK53" s="17"/>
-      <c r="CL53" s="17"/>
-      <c r="CM53" s="17"/>
-      <c r="CN53" s="17"/>
-      <c r="CO53" s="17"/>
-      <c r="CP53" s="17"/>
-      <c r="CQ53" s="17"/>
-      <c r="CR53" s="17"/>
-      <c r="CS53" s="17"/>
-      <c r="CT53" s="17"/>
-      <c r="CU53" s="17"/>
-      <c r="CV53" s="17"/>
-      <c r="CW53" s="17"/>
-      <c r="CX53" s="17"/>
-      <c r="CY53" s="17"/>
-      <c r="CZ53" s="17"/>
-      <c r="DA53" s="17"/>
-      <c r="DB53" s="17"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="CV4:DB4"/>
@@ -8737,9 +8621,6 @@
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D19">
@@ -8756,12 +8637,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM6:DB6 I6:BL53 BM8:DB53 I5:DB5">
+  <conditionalFormatting sqref="BM6:DB6 I5:DB5 I6:BL52 BM8:DB52">
     <cfRule type="expression" dxfId="5" priority="37">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL53 BM8:DB53">
+  <conditionalFormatting sqref="I7:BL52 BM8:DB52">
     <cfRule type="expression" dxfId="4" priority="31">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -8769,7 +8650,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D35">
+  <conditionalFormatting sqref="D30:D34">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8783,7 +8664,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D39">
+  <conditionalFormatting sqref="D35:D38">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8868,7 +8749,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D30:D35</xm:sqref>
+          <xm:sqref>D30:D34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{881682AF-F74D-495F-97BB-62AC893D6F55}">
@@ -8883,7 +8764,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36:D39</xm:sqref>
+          <xm:sqref>D35:D38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{08B863AC-BB4A-4D00-9275-CB6968C2EF23}">
@@ -8926,11 +8807,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DB53"/>
+  <dimension ref="A1:DB52"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:F23"/>
+      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8951,11 +8832,11 @@
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="B1" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="H1" s="1"/>
@@ -8965,10 +8846,10 @@
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="103"/>
+      <c r="B2" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="94"/>
       <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8976,164 +8857,164 @@
         <v>2</v>
       </c>
       <c r="B3" s="71"/>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="95">
+      <c r="D3" s="101"/>
+      <c r="E3" s="96">
         <f>DATE(2022,9,15)</f>
         <v>44819</v>
       </c>
-      <c r="F3" s="95"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:106" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="102"/>
+      <c r="D4" s="103"/>
       <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="96" t="s">
+      <c r="I4" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="96" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="98"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="98"/>
-      <c r="W4" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="92">
+      <c r="X4" s="98"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
         <v>44837</v>
       </c>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="93"/>
-      <c r="AJ4" s="94"/>
-      <c r="AK4" s="92">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
         <v>44844</v>
       </c>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="93"/>
-      <c r="AN4" s="93"/>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="94"/>
-      <c r="AR4" s="92">
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
         <v>44851</v>
       </c>
-      <c r="AS4" s="93"/>
-      <c r="AT4" s="93"/>
-      <c r="AU4" s="93"/>
-      <c r="AV4" s="93"/>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="94"/>
-      <c r="AY4" s="92">
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
         <v>44858</v>
       </c>
-      <c r="AZ4" s="93"/>
-      <c r="BA4" s="93"/>
-      <c r="BB4" s="93"/>
-      <c r="BC4" s="93"/>
-      <c r="BD4" s="93"/>
-      <c r="BE4" s="94"/>
-      <c r="BF4" s="92">
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
         <v>44865</v>
       </c>
-      <c r="BG4" s="93"/>
-      <c r="BH4" s="93"/>
-      <c r="BI4" s="93"/>
-      <c r="BJ4" s="93"/>
-      <c r="BK4" s="93"/>
-      <c r="BL4" s="94"/>
-      <c r="BM4" s="92">
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="91">
         <f>BM5</f>
         <v>44872</v>
       </c>
-      <c r="BN4" s="93"/>
-      <c r="BO4" s="93"/>
-      <c r="BP4" s="93"/>
-      <c r="BQ4" s="93"/>
-      <c r="BR4" s="93"/>
-      <c r="BS4" s="94"/>
-      <c r="BT4" s="92">
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="92"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="91">
         <f>BT5</f>
         <v>44879</v>
       </c>
-      <c r="BU4" s="93"/>
-      <c r="BV4" s="93"/>
-      <c r="BW4" s="93"/>
-      <c r="BX4" s="93"/>
-      <c r="BY4" s="93"/>
-      <c r="BZ4" s="94"/>
-      <c r="CA4" s="92">
+      <c r="BU4" s="92"/>
+      <c r="BV4" s="92"/>
+      <c r="BW4" s="92"/>
+      <c r="BX4" s="92"/>
+      <c r="BY4" s="92"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="91">
         <f>CA5</f>
         <v>44886</v>
       </c>
-      <c r="CB4" s="93"/>
-      <c r="CC4" s="93"/>
-      <c r="CD4" s="93"/>
-      <c r="CE4" s="93"/>
-      <c r="CF4" s="93"/>
-      <c r="CG4" s="94"/>
-      <c r="CH4" s="92">
+      <c r="CB4" s="92"/>
+      <c r="CC4" s="92"/>
+      <c r="CD4" s="92"/>
+      <c r="CE4" s="92"/>
+      <c r="CF4" s="92"/>
+      <c r="CG4" s="93"/>
+      <c r="CH4" s="91">
         <f>CH5</f>
         <v>44893</v>
       </c>
-      <c r="CI4" s="93"/>
-      <c r="CJ4" s="93"/>
-      <c r="CK4" s="93"/>
-      <c r="CL4" s="93"/>
-      <c r="CM4" s="93"/>
-      <c r="CN4" s="94"/>
-      <c r="CO4" s="92">
+      <c r="CI4" s="92"/>
+      <c r="CJ4" s="92"/>
+      <c r="CK4" s="92"/>
+      <c r="CL4" s="92"/>
+      <c r="CM4" s="92"/>
+      <c r="CN4" s="93"/>
+      <c r="CO4" s="91">
         <f>CO5</f>
         <v>44900</v>
       </c>
-      <c r="CP4" s="93"/>
-      <c r="CQ4" s="93"/>
-      <c r="CR4" s="93"/>
-      <c r="CS4" s="93"/>
-      <c r="CT4" s="93"/>
-      <c r="CU4" s="94"/>
-      <c r="CV4" s="92">
+      <c r="CP4" s="92"/>
+      <c r="CQ4" s="92"/>
+      <c r="CR4" s="92"/>
+      <c r="CS4" s="92"/>
+      <c r="CT4" s="92"/>
+      <c r="CU4" s="93"/>
+      <c r="CV4" s="91">
         <f>CV5</f>
         <v>44907</v>
       </c>
-      <c r="CW4" s="93"/>
-      <c r="CX4" s="93"/>
-      <c r="CY4" s="93"/>
-      <c r="CZ4" s="93"/>
-      <c r="DA4" s="93"/>
-      <c r="DB4" s="94"/>
+      <c r="CW4" s="92"/>
+      <c r="CX4" s="92"/>
+      <c r="CY4" s="92"/>
+      <c r="CZ4" s="92"/>
+      <c r="DA4" s="92"/>
+      <c r="DB4" s="93"/>
     </row>
     <row r="5" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
@@ -9555,11 +9436,11 @@
         <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" ref="I6:BT6" si="9">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -10026,7 +9907,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="8"/>
@@ -10034,7 +9915,7 @@
       <c r="F8" s="46"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="str">
-        <f t="shared" ref="H8:H53" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H52" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="17"/>
@@ -10141,10 +10022,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="35" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>41</v>
       </c>
       <c r="D9" s="9">
         <v>0</v>
@@ -10266,10 +10147,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
@@ -10389,10 +10270,10 @@
     <row r="11" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="9">
         <v>0</v>
@@ -10512,10 +10393,10 @@
     <row r="12" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="9">
         <v>0</v>
@@ -10635,10 +10516,10 @@
     <row r="13" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -10760,7 +10641,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="10"/>
@@ -10873,10 +10754,10 @@
     <row r="15" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="70" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>51</v>
       </c>
       <c r="D15" s="11">
         <v>1</v>
@@ -10996,10 +10877,10 @@
     <row r="16" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16" s="63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="11">
         <v>1</v>
@@ -11119,10 +11000,10 @@
     <row r="17" spans="1:106" s="2" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="11">
         <v>0.75</v>
@@ -11242,10 +11123,10 @@
     <row r="18" spans="1:106" s="2" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="11">
         <v>0.9</v>
@@ -11365,10 +11246,10 @@
     <row r="19" spans="1:106" s="2" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="11">
         <v>0.9</v>
@@ -11488,7 +11369,7 @@
     <row r="20" spans="1:106" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="39"/>
       <c r="D20" s="14"/>
@@ -11598,10 +11479,10 @@
     <row r="21" spans="1:106" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
       <c r="B21" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="15">
         <v>0</v>
@@ -11718,10 +11599,10 @@
     <row r="22" spans="1:106" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="15">
         <v>0</v>
@@ -11838,10 +11719,10 @@
     <row r="23" spans="1:106" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="15">
         <v>0</v>
@@ -11960,7 +11841,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="12"/>
@@ -12073,10 +11954,10 @@
     <row r="25" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="13">
         <v>0</v>
@@ -12196,10 +12077,10 @@
     <row r="26" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="13">
         <v>0</v>
@@ -12319,10 +12200,10 @@
     <row r="27" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="13">
         <v>0</v>
@@ -12442,7 +12323,7 @@
     <row r="28" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
       <c r="B28" s="65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="13">
@@ -12563,7 +12444,7 @@
     <row r="29" spans="1:106" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29" s="65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="38"/>
       <c r="D29" s="13">
@@ -12686,7 +12567,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="73"/>
       <c r="D30" s="74"/>
@@ -12801,7 +12682,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="78"/>
       <c r="D31" s="79">
@@ -12921,7 +12802,7 @@
     </row>
     <row r="32" spans="1:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="77" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="79">
@@ -13041,7 +12922,7 @@
     </row>
     <row r="33" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="78"/>
       <c r="D33" s="79">
@@ -13161,7 +13042,7 @@
     </row>
     <row r="34" spans="2:106" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="78"/>
       <c r="D34" s="79">
@@ -13280,21 +13161,17 @@
       <c r="DB34" s="17"/>
     </row>
     <row r="35" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="77"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="79">
-        <v>0</v>
-      </c>
-      <c r="E35" s="80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="80" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="16" t="e">
+      <c r="H35" s="16" t="str">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -13396,17 +13273,25 @@
       <c r="DB35" s="17"/>
     </row>
     <row r="36" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="81" t="s">
+      <c r="B36" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="85"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="88">
+        <v>0</v>
+      </c>
+      <c r="E36" s="89">
+        <f>CA5</f>
+        <v>44886</v>
+      </c>
+      <c r="F36" s="89">
+        <f>CG5</f>
+        <v>44892</v>
+      </c>
       <c r="G36" s="16"/>
-      <c r="H36" s="16" t="str">
+      <c r="H36" s="16">
         <f t="shared" si="11"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -13508,25 +13393,10 @@
       <c r="DB36" s="17"/>
     </row>
     <row r="37" spans="2:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="88">
-        <v>0</v>
-      </c>
-      <c r="E37" s="89">
-        <f>CA5</f>
-        <v>44886</v>
-      </c>
-      <c r="F37" s="89">
-        <f>CG5</f>
-        <v>44892</v>
-      </c>
       <c r="G37" s="16"/>
-      <c r="H37" s="16">
+      <c r="H37" s="16" t="str">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
@@ -15202,120 +15072,8 @@
       <c r="DA52" s="17"/>
       <c r="DB52" s="17"/>
     </row>
-    <row r="53" spans="7:106" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="16"/>
-      <c r="H53" s="16" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="19"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="19"/>
-      <c r="W53" s="19"/>
-      <c r="X53" s="19"/>
-      <c r="Y53" s="19"/>
-      <c r="Z53" s="19"/>
-      <c r="AA53" s="19"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="19"/>
-      <c r="AD53" s="19"/>
-      <c r="AE53" s="19"/>
-      <c r="AF53" s="19"/>
-      <c r="AG53" s="19"/>
-      <c r="AH53" s="19"/>
-      <c r="AI53" s="19"/>
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-      <c r="AL53" s="19"/>
-      <c r="AM53" s="19"/>
-      <c r="AN53" s="19"/>
-      <c r="AO53" s="19"/>
-      <c r="AP53" s="19"/>
-      <c r="AQ53" s="19"/>
-      <c r="AR53" s="19"/>
-      <c r="AS53" s="19"/>
-      <c r="AT53" s="19"/>
-      <c r="AU53" s="19"/>
-      <c r="AV53" s="19"/>
-      <c r="AW53" s="19"/>
-      <c r="AX53" s="19"/>
-      <c r="AY53" s="19"/>
-      <c r="AZ53" s="19"/>
-      <c r="BA53" s="19"/>
-      <c r="BB53" s="19"/>
-      <c r="BC53" s="19"/>
-      <c r="BD53" s="19"/>
-      <c r="BE53" s="19"/>
-      <c r="BF53" s="19"/>
-      <c r="BG53" s="19"/>
-      <c r="BH53" s="19"/>
-      <c r="BI53" s="19"/>
-      <c r="BJ53" s="19"/>
-      <c r="BK53" s="19"/>
-      <c r="BL53" s="19"/>
-      <c r="BM53" s="17"/>
-      <c r="BN53" s="17"/>
-      <c r="BO53" s="17"/>
-      <c r="BP53" s="17"/>
-      <c r="BQ53" s="17"/>
-      <c r="BR53" s="17"/>
-      <c r="BS53" s="17"/>
-      <c r="BT53" s="17"/>
-      <c r="BU53" s="17"/>
-      <c r="BV53" s="17"/>
-      <c r="BW53" s="17"/>
-      <c r="BX53" s="17"/>
-      <c r="BY53" s="17"/>
-      <c r="BZ53" s="17"/>
-      <c r="CA53" s="17"/>
-      <c r="CB53" s="17"/>
-      <c r="CC53" s="17"/>
-      <c r="CD53" s="17"/>
-      <c r="CE53" s="17"/>
-      <c r="CF53" s="17"/>
-      <c r="CG53" s="17"/>
-      <c r="CH53" s="17"/>
-      <c r="CI53" s="17"/>
-      <c r="CJ53" s="17"/>
-      <c r="CK53" s="17"/>
-      <c r="CL53" s="17"/>
-      <c r="CM53" s="17"/>
-      <c r="CN53" s="17"/>
-      <c r="CO53" s="17"/>
-      <c r="CP53" s="17"/>
-      <c r="CQ53" s="17"/>
-      <c r="CR53" s="17"/>
-      <c r="CS53" s="17"/>
-      <c r="CT53" s="17"/>
-      <c r="CU53" s="17"/>
-      <c r="CV53" s="17"/>
-      <c r="CW53" s="17"/>
-      <c r="CX53" s="17"/>
-      <c r="CY53" s="17"/>
-      <c r="CZ53" s="17"/>
-      <c r="DA53" s="17"/>
-      <c r="DB53" s="17"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -15328,9 +15086,16 @@
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D37">
+  <conditionalFormatting sqref="D7:D36">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15344,12 +15109,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:DB6 I5:BL23 BM8:DB23 I24:DB53">
+  <conditionalFormatting sqref="BM5:DB6 I5:BL23 BM8:DB23 I24:DB52">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL23 BM8:DB23 I24:DB53">
+  <conditionalFormatting sqref="I7:BL23 BM8:DB23 I24:DB52">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -15385,7 +15150,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D37</xm:sqref>
+          <xm:sqref>D7:D36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15408,79 +15173,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:2" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="27"/>
     </row>
     <row r="4" spans="1:2" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="20" customFormat="1" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="20" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="20" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -15497,35 +15262,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15813,27 +15549,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15852,4 +15597,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificación en el progreso de las actividades
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EE6070-D617-48E5-B7FF-FDE278AC0077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2E017D-8434-4810-97AD-8AF1AC66280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="591" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="591" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeacion (tiempo real)" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -315,6 +315,15 @@
   </si>
   <si>
     <t>Subida de todos los archivos faltantes al repositorio</t>
+  </si>
+  <si>
+    <t>Hernández Hernández Pedro Daniel y Marín  Barrera Jorge Jair</t>
+  </si>
+  <si>
+    <t>Marin Barrera Jorge Jair</t>
+  </si>
+  <si>
+    <t>Hernandez Hernandez Pedro Daniel y Marín Barrera Jorge Jair</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1126,7 @@
     <xf numFmtId="0" fontId="6" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1417,6 +1426,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="46" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2301,9 +2313,9 @@
   </sheetPr>
   <dimension ref="A1:DB52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4498,7 +4510,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="11">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E17" s="58">
         <f>E16</f>
@@ -4979,10 +4991,10 @@
         <v>59</v>
       </c>
       <c r="C21" s="90" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="D21" s="15">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E21" s="59">
         <f>BM5</f>
@@ -5102,10 +5114,10 @@
         <v>61</v>
       </c>
       <c r="C22" s="90" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D22" s="15">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E22" s="59">
         <f>BM5</f>
@@ -5225,7 +5237,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D23" s="15">
         <v>0</v>
@@ -5466,20 +5478,20 @@
         <v>40</v>
       </c>
       <c r="D25" s="13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="51">
-        <f>E11+16</f>
-        <v>44841</v>
+        <f>CA5</f>
+        <v>44886</v>
       </c>
       <c r="F25" s="51">
-        <f>E25+7</f>
-        <v>44848</v>
+        <f>E25+23</f>
+        <v>44909</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7">
         <f t="shared" si="42"/>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
@@ -5592,17 +5604,17 @@
         <v>0</v>
       </c>
       <c r="E26" s="51">
-        <f>F25+1</f>
-        <v>44849</v>
+        <f>CA5</f>
+        <v>44886</v>
       </c>
       <c r="F26" s="51">
-        <f>E26+3</f>
-        <v>44852</v>
+        <f>E25+23</f>
+        <v>44909</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7">
         <f t="shared" si="42"/>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
@@ -5715,17 +5727,17 @@
         <v>0</v>
       </c>
       <c r="E27" s="51">
-        <f>E26+4</f>
-        <v>44853</v>
+        <f>CA5</f>
+        <v>44886</v>
       </c>
       <c r="F27" s="51">
-        <f>E27+8</f>
-        <v>44861</v>
+        <f>E25+23</f>
+        <v>44909</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7">
         <f t="shared" si="42"/>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
@@ -5831,22 +5843,24 @@
       <c r="B28" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="38"/>
+      <c r="C28" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="D28" s="13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E28" s="51">
-        <f>F27+1</f>
-        <v>44862</v>
+        <f>CA5</f>
+        <v>44886</v>
       </c>
       <c r="F28" s="51">
-        <f>E28+9</f>
-        <v>44871</v>
+        <f>E25+23</f>
+        <v>44909</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7">
         <f t="shared" si="42"/>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -5952,22 +5966,24 @@
       <c r="B29" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="38"/>
+      <c r="C29" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="D29" s="13">
         <v>0</v>
       </c>
       <c r="E29" s="51">
-        <f>BG7</f>
-        <v>0</v>
+        <f>CA5</f>
+        <v>44886</v>
       </c>
       <c r="F29" s="51">
-        <f>E29+1</f>
-        <v>1</v>
+        <f>E25+23</f>
+        <v>44909</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7">
         <f t="shared" si="42"/>
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
@@ -6190,7 +6206,9 @@
       <c r="B31" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="78"/>
+      <c r="C31" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="D31" s="79">
         <v>0</v>
       </c>
@@ -6310,7 +6328,9 @@
       <c r="B32" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="D32" s="79">
         <v>0</v>
       </c>
@@ -6430,7 +6450,9 @@
       <c r="B33" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="78"/>
+      <c r="C33" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="D33" s="79">
         <v>0</v>
       </c>
@@ -6550,7 +6572,9 @@
       <c r="B34" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="78"/>
+      <c r="C34" s="104" t="s">
+        <v>40</v>
+      </c>
       <c r="D34" s="79">
         <v>0</v>
       </c>
@@ -6782,7 +6806,9 @@
       <c r="B36" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="87"/>
+      <c r="C36" s="87" t="s">
+        <v>40</v>
+      </c>
       <c r="D36" s="88">
         <v>0</v>
       </c>
@@ -7014,7 +7040,9 @@
       <c r="B38" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="40"/>
+      <c r="C38" s="40" t="s">
+        <v>40</v>
+      </c>
       <c r="D38" s="15">
         <v>0</v>
       </c>
@@ -8602,11 +8630,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:D1"/>
@@ -8621,6 +8644,11 @@
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D19">
@@ -15074,6 +15102,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -15086,13 +15121,6 @@
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D36">
@@ -15262,6 +15290,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15549,36 +15606,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15597,24 +15645,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>